<commit_message>
jupyter notebook amiris, NEW config electrolyzer fileld map
</commit_message>
<xml_diff>
--- a/data/Analysis/Amiris-Competes_analysis.xlsx
+++ b/data/Analysis/Amiris-Competes_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C36CB6-6970-4AED-B264-DC1658D0D308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10EC430-5CD7-42F4-A833-89296770AEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3772C9F9-3F70-4642-9AE3-8682248B1B42}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{3772C9F9-3F70-4642-9AE3-8682248B1B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Imports</t>
   </si>
@@ -542,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,7 +553,7 @@
   <dimension ref="B1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,7 +942,7 @@
         <v>0.9806487616250783</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" si="4"/>
+        <f>O2/$T2</f>
         <v>0.3681862611687623</v>
       </c>
       <c r="P8" s="2">

</xml_diff>